<commit_message>
up dataset for Ivan and ref
</commit_message>
<xml_diff>
--- a/Book 1.xlsx
+++ b/Book 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lipen\PycharmProjects\My_classifier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0FACBE-AB3E-4F43-BFA6-870C0633D917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF45AAAD-9AA3-4A23-9AD3-CD3F56E2AB2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{03F764E3-85F1-49B5-8786-945FC52AAEF2}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1909" uniqueCount="738">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1969" uniqueCount="762">
   <si>
     <t xml:space="preserve"> @ АЗС</t>
   </si>
@@ -2246,6 +2246,78 @@
   </si>
   <si>
     <t>Где можно остановиться на отдых на М1 перед городом с рестораном и кафе? @ Отдых</t>
+  </si>
+  <si>
+    <t>Где на трассе М1 можно найти ресторан с национальной кухней? @ Еда</t>
+  </si>
+  <si>
+    <t>Есть ли кафе на трассе М10, где подают быстрые закуски? @ Еда</t>
+  </si>
+  <si>
+    <t>Какие рестораны на М4 предлагают вегетарианское меню? @ Еда</t>
+  </si>
+  <si>
+    <t>Где на М5 можно найти кафе с домашней выпечкой? @ Еда</t>
+  </si>
+  <si>
+    <t>Можно ли найти на М2 место, где готовят свежие морепродукты? @ Еда</t>
+  </si>
+  <si>
+    <t>Подскажите рестораны на М6, где можно попробовать местные деликатесы? @ Еда</t>
+  </si>
+  <si>
+    <t>Есть ли на М8 кафе с детским меню и игровой зоной? @ Еда</t>
+  </si>
+  <si>
+    <t>Где на М11 можно найти ресторан с видом на озеро? @ Еда</t>
+  </si>
+  <si>
+    <t>Какие рестораны на М3 предлагают бизнес-ланчи? @ Еда</t>
+  </si>
+  <si>
+    <t>Где на М7 можно найти кафе с домашней кухней? @ Еда</t>
+  </si>
+  <si>
+    <t>Есть ли на М1 рестораны с авторской кухней? @ Еда</t>
+  </si>
+  <si>
+    <t>Где на М10 можно найти кафе с быстрым обслуживанием? @ Еда</t>
+  </si>
+  <si>
+    <t>Подскажите рестораны на М4, где можно попробовать местные специализации? @ Еда</t>
+  </si>
+  <si>
+    <t>Где на М5 можно найти кафе с домашними десертами? @ Еда</t>
+  </si>
+  <si>
+    <t>Можно ли найти на М2 место, где готовят свежие овощи и фрукты? @ Еда</t>
+  </si>
+  <si>
+    <t>Есть ли на М6 кафе с традиционными напитками? @ Еда</t>
+  </si>
+  <si>
+    <t>Где на М8 можно найти ресторан с дегустацией местных вин? @ Еда</t>
+  </si>
+  <si>
+    <t>Какие рестораны на М11 предлагают морепродукты? @ Еда</t>
+  </si>
+  <si>
+    <t>Где на М3 можно найти кафе с домашними обедами? @ Еда</t>
+  </si>
+  <si>
+    <t>Подскажите рестораны на М7, где можно попробовать блюда из региональной кухни? @ Еда</t>
+  </si>
+  <si>
+    <t>Есть ли на М1 рестораны с местными деликатесами? @ Еда</t>
+  </si>
+  <si>
+    <t>Где на М10 можно найти кафе с меню для диетического питания? @ Еда</t>
+  </si>
+  <si>
+    <t>Подскажите рестораны на М4, где можно попробовать экзотическую кухню? @ Еда</t>
+  </si>
+  <si>
+    <t>Где на М5 можно найти кафе с домашними пирогами? @ Еда</t>
   </si>
 </sst>
 </file>
@@ -2615,10 +2687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9C13D30-FAD8-4B25-BC5F-166A891BC747}">
-  <dimension ref="A1:C1539"/>
+  <dimension ref="A1:C1628"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1487" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C1500" sqref="C1500:C1539"/>
+    <sheetView tabSelected="1" topLeftCell="B1595" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C1629" sqref="C1629"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13113,6 +13185,306 @@
         <v>708</v>
       </c>
     </row>
+    <row r="1540" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1540" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="1541" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1541" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="1542" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1542" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="1543" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1543" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="1544" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1544" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="1545" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1545" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="1546" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1546" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="1547" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1547" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="1548" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1548" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="1549" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1549" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="1550" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1550" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="1551" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1551" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="1552" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1552" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="1553" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1553" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="1554" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1554" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="1555" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1555" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="1556" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1556" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="1557" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1557" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="1558" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1558" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="1559" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1559" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="1560" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1560" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="1561" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1561" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="1562" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1562" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="1563" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1563" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="1564" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1564" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="1565" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1565" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="1566" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1566" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="1567" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1567" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="1568" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1568" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="1569" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1569" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="1570" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1570" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="1572" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1572" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="1574" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1574" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="1576" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1576" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="1578" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1578" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="1580" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1580" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="1582" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1582" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="1584" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1584" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="1586" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1586" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="1588" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1588" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="1590" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1590" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="1592" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1592" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="1594" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1594" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="1596" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1596" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="1598" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1598" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="1600" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1600" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="1602" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1602" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="1604" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1604" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="1606" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1606" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="1608" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1608" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="1610" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1610" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="1612" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1612" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="1614" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1614" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="1616" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1616" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="1618" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1618" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="1620" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1620" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="1622" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1622" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="1624" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1624" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="1626" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1626" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="1628" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1628" t="s">
+        <v>757</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:C470">
     <sortCondition ref="A1:A470"/>

</xml_diff>